<commit_message>
-Adding wire to board terminal block
</commit_message>
<xml_diff>
--- a/Rleased/BOM/H05R0.xlsx
+++ b/Rleased/BOM/H05R0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H05R0x-Hardware\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A65149E-37D4-400A-AC16-D6277063A115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48358F3-6F52-4C32-B2FF-580BCC66C2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H05R0" sheetId="1" r:id="rId1"/>
@@ -1728,7 +1728,7 @@
   <dimension ref="A2:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2351,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
-Correcting the placement of the additional junction and including it in the Bill of Materials (BOM).
</commit_message>
<xml_diff>
--- a/Rleased/BOM/H05R0.xlsx
+++ b/Rleased/BOM/H05R0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H05R0x-Hardware\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48358F3-6F52-4C32-B2FF-580BCC66C2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2C4458-9C80-41AE-B460-F71F384ADE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="196">
   <si>
     <t>Description</t>
   </si>
@@ -602,6 +602,18 @@
   </si>
   <si>
     <t xml:space="preserve">1s Lipo charger w/ USB-C  (H05R0) </t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>2pin Terminal Block; Printed Circuit; 10 A; 160 V; 3.5 mm; 2; 3.5 mm; 1.2 mm; M2; PA</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>https://octopart.com/1984617-phoenix+contact-58834?r=sp&amp;s=Ef_UaV1JSFmY0wggQyN1Mw</t>
   </si>
 </sst>
 </file>
@@ -1725,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1931,41 +1943,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1984617</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B15" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C15" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E15" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="F14" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>156</v>
       </c>
       <c r="F15" s="17">
         <v>1</v>
@@ -1973,79 +1985,79 @@
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B17" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C17" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E17" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="F16" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="F17" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B18" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C18" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F18" s="17">
         <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="17">
-        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="F19" s="17">
         <v>2</v>
@@ -2053,99 +2065,99 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>61</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>160</v>
+        <v>79</v>
       </c>
       <c r="F21" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="F22" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>161</v>
+        <v>80</v>
       </c>
       <c r="F23" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F24" s="17">
         <v>1</v>
@@ -2153,19 +2165,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="F25" s="17">
         <v>1</v>
@@ -2173,99 +2185,99 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B27" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C27" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D27" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="F27" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C28" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>186</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="F28" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="F29" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B30" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C30" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D30" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>164</v>
-      </c>
-      <c r="F29" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="F30" s="17">
         <v>1</v>
@@ -2273,79 +2285,79 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B32" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C32" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D32" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E32" s="16" t="s">
         <v>19</v>
-      </c>
-      <c r="F31" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>87</v>
       </c>
       <c r="F32" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>165</v>
+        <v>87</v>
       </c>
       <c r="F33" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F34" s="17">
         <v>1</v>
@@ -2353,19 +2365,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F35" s="17">
         <v>1</v>
@@ -2373,59 +2385,59 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F36" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B37" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C37" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D37" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E37" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="F36" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="F37" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B38" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D38" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E38" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="F37" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>84</v>
       </c>
       <c r="F38" s="17">
         <v>1</v>
@@ -2433,19 +2445,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>149</v>
+        <v>41</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>169</v>
+        <v>84</v>
       </c>
       <c r="F39" s="17">
         <v>1</v>
@@ -2453,19 +2465,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="F40" s="17">
         <v>1</v>
@@ -2473,121 +2485,141 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B42" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C42" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D42" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E42" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="F41" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="F42" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B43" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D43" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E43" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="F43" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B44" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C44" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D44" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E44" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="F43" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="F44" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B45" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C45" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D45" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E45" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="F44" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="F45" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B46" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C46" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D46" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E46" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="F45" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="F46" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B47" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C47" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D47" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E47" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="17">
+      <c r="F47" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2598,20 +2630,20 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E19" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E20" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E25" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E27" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E30" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E32" r:id="rId11" display="https://octopart.com/grm21br61h106ke43k-murata-106705599?r=sp" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="E31" r:id="rId12" xr:uid="{CA2BC9B7-037F-4782-ACB8-2D8F29264691}"/>
-    <hyperlink ref="E38" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E37" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E23" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E26" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E28" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E31" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E33" r:id="rId11" display="https://octopart.com/grm21br61h106ke43k-murata-106705599?r=sp" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E32" r:id="rId12" xr:uid="{CA2BC9B7-037F-4782-ACB8-2D8F29264691}"/>
+    <hyperlink ref="E39" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E38" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>

</xml_diff>

<commit_message>
-Update the logo and add TVS
</commit_message>
<xml_diff>
--- a/Rleased/BOM/H05R0.xlsx
+++ b/Rleased/BOM/H05R0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H05R0x-Hardware\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2C4458-9C80-41AE-B460-F71F384ADE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF6F91A-D1E8-449D-888B-664535AEB853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="201">
   <si>
     <t>Description</t>
   </si>
@@ -614,6 +614,21 @@
   </si>
   <si>
     <t>https://octopart.com/1984617-phoenix+contact-58834?r=sp&amp;s=Ef_UaV1JSFmY0wggQyN1Mw</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3,3V 10,9V SOD323</t>
+  </si>
+  <si>
+    <t>CDSOD323-T03SC</t>
+  </si>
+  <si>
+    <t>BOURNS INC</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cdsod323-t03sc-bourns-10487153?r=sp</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
 </sst>
 </file>
@@ -1737,10 +1752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G47"/>
+  <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2505,39 +2520,39 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F42" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B43" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D43" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E43" s="16" t="s">
         <v>170</v>
-      </c>
-      <c r="F42" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="F43" s="17">
         <v>1</v>
@@ -2545,19 +2560,19 @@
     </row>
     <row r="44" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>142</v>
+        <v>36</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>171</v>
+        <v>40</v>
       </c>
       <c r="F44" s="17">
         <v>1</v>
@@ -2565,19 +2580,19 @@
     </row>
     <row r="45" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F45" s="17">
         <v>1</v>
@@ -2585,41 +2600,61 @@
     </row>
     <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="F46" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B47" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C47" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D47" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E47" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="F46" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="F47" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B48" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C48" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D48" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E48" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="17">
+      <c r="F48" s="17">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-New Version (1b), reviewed and finished - adding the charging detection & current measurement circuit
</commit_message>
<xml_diff>
--- a/Rleased/BOM/H05R0.xlsx
+++ b/Rleased/BOM/H05R0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H05R0x-Hardware\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF6F91A-D1E8-449D-888B-664535AEB853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC05B3A5-A523-4D31-8921-5D6A35488D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="235">
   <si>
     <t>Description</t>
   </si>
@@ -73,21 +73,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>KEMET</t>
-  </si>
-  <si>
     <t>Murata</t>
   </si>
   <si>
     <t>Panasonic</t>
   </si>
   <si>
-    <t>10TPU4R7MSI</t>
-  </si>
-  <si>
-    <t>https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp</t>
-  </si>
-  <si>
     <t>Vishay</t>
   </si>
   <si>
@@ -112,9 +103,6 @@
     <t>https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp</t>
   </si>
   <si>
-    <t>YAGEO [VR]</t>
-  </si>
-  <si>
     <t>ERJ-3GEYJ271V</t>
   </si>
   <si>
@@ -136,21 +124,12 @@
     <t>https://octopart.com/mmz1608y300bta00-tdk-7906990?r=sp</t>
   </si>
   <si>
-    <t>STM32G0B1CEU6N</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
-    <t>MCU 32-Bit ARM Cortex-M0+ RISC 512kByte Flash 1.7V to 3.6V 48-Pin UFQFPN Tray</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
-    <t>https://octopart.com/stm32g0b1ceu6n-stmicroelectronics-116364672?r=sp</t>
-  </si>
-  <si>
     <t>VLMS1300-GS08</t>
   </si>
   <si>
@@ -166,9 +145,6 @@
     <t>https://octopart.com/cstne8m00g550000r0-murata-91406934?r=sp</t>
   </si>
   <si>
-    <t>CAP TANT 4.7 UF 10V 20% 0805</t>
-  </si>
-  <si>
     <t>CAP CER 1 UF 16V X7R 0805</t>
   </si>
   <si>
@@ -181,33 +157,15 @@
     <t>Hexabitz Modules</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C0603C104K8RACTU</t>
-  </si>
-  <si>
     <t>YAGEO</t>
   </si>
   <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
     <t>R</t>
   </si>
   <si>
-    <t>RES SMD 0.0OHM JUMPER 1/10W 0603</t>
-  </si>
-  <si>
-    <t>RC0603JR-070RL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp</t>
-  </si>
-  <si>
     <t xml:space="preserve"> SWD</t>
   </si>
   <si>
@@ -274,30 +232,9 @@
     <t>https://octopart.com/cc0603krnpo9bn102-yageo-65850404?r=sp</t>
   </si>
   <si>
-    <t>CAP CER 0.1 UF 10V 10% X7R 0603</t>
-  </si>
-  <si>
-    <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp</t>
-  </si>
-  <si>
     <t>https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp</t>
   </si>
   <si>
-    <t>CAP CER 10UF 10V X5R 0603</t>
-  </si>
-  <si>
-    <t>GRM188R61A106KE69D</t>
-  </si>
-  <si>
-    <t>https://octopart.com/grm188r61a106ke69d-murata-22851381?r=ap&amp;s=o9t4ILLiSny6rfdd0oM5Kg</t>
-  </si>
-  <si>
-    <t>C11, C15</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -310,12 +247,6 @@
     <t>Susumu</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R3, R11, R21</t>
-  </si>
-  <si>
     <t>NCP18XH103F03RB</t>
   </si>
   <si>
@@ -331,9 +262,6 @@
     <t>RES 10 OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>R10, R18</t>
-  </si>
-  <si>
     <t>CAP CER 0.022UF 50V X7R 0603</t>
   </si>
   <si>
@@ -346,24 +274,9 @@
     <t>C18</t>
   </si>
   <si>
-    <t>CL10A476MQ8QRNC</t>
-  </si>
-  <si>
-    <t>CAP CER 47UF 6.3V X5R 0603</t>
-  </si>
-  <si>
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>T491B226K010AT</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>R19</t>
   </si>
   <si>
@@ -373,9 +286,6 @@
     <t>RC0603FR-102ML</t>
   </si>
   <si>
-    <t>EXT_TH_J</t>
-  </si>
-  <si>
     <t>2 Position Total Single Row 2.54 mm Pitch Straight Male Thru-Hole Header</t>
   </si>
   <si>
@@ -394,27 +304,6 @@
     <t>GRM188R71A474KA61D</t>
   </si>
   <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>GRM187R61A226ME15D</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 22 uF 10 VDC 20% 0603 X5R</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>CRCW0603665KFKEAC</t>
-  </si>
-  <si>
-    <t>RES 665K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>Vishay / Dale</t>
-  </si>
-  <si>
     <t>BAT_J</t>
   </si>
   <si>
@@ -427,24 +316,9 @@
     <t>JST</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>DFE2HCAH1R0MJ0L</t>
-  </si>
-  <si>
-    <t>Power Inductors - SMD 1 UH 20%</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
-    <t>ECH8693R-TL-W</t>
-  </si>
-  <si>
-    <t>MOSFET N-CH Pwr MOSFET 24V 14A 7mOhm</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -463,39 +337,12 @@
     <t>Analog Devices / Maxim Integrated</t>
   </si>
   <si>
-    <t>Switching Voltage Regulators 1.5-A output current, high power density buck-boost converter</t>
-  </si>
-  <si>
-    <t>TPS631000DRLR</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
-    <t>TVS DIODE 5VWM 12.5VC SOD523</t>
-  </si>
-  <si>
-    <t>UCLAMP0501H.TCT</t>
-  </si>
-  <si>
-    <t>Semtech</t>
-  </si>
-  <si>
-    <t>UJC-HP-G-SMT-TR</t>
-  </si>
-  <si>
-    <t>CUI Devices</t>
-  </si>
-  <si>
-    <t>USB Connectors USB jack, C type, power only, 8 pin, horizonal, gold flash plating, surface mount</t>
-  </si>
-  <si>
     <t>USB_C</t>
   </si>
   <si>
-    <t>https://octopart.com/ujc-hp-g-smt-tr-cui+devices-113163754?r=sp</t>
-  </si>
-  <si>
     <t>https://octopart.com/krl1220e-m-r010-f-t5-susumu-24927387?r=sp</t>
   </si>
   <si>
@@ -511,9 +358,6 @@
     <t>https://octopart.com/ncp18xh103f03rb-murata-746135?r=sp</t>
   </si>
   <si>
-    <t>https://octopart.com/crcw0603665kfkeac-vishay-22248099?r=sp</t>
-  </si>
-  <si>
     <t>https://octopart.com/rc0603fr-102ml-yageo-16255871?r=sp</t>
   </si>
   <si>
@@ -523,39 +367,12 @@
     <t>https://octopart.com/grm188r71a474ka61d-murata-11812018?r=sp</t>
   </si>
   <si>
-    <t>https://octopart.com/grm187r61a226me15d-murata-71221003?r=sp</t>
-  </si>
-  <si>
-    <t>https://octopart.com/t491b226k010at-kemet-148836?r=sp</t>
-  </si>
-  <si>
-    <t>https://octopart.com/cl10a476mq8qrnc-samsung-71808721?r=sp</t>
-  </si>
-  <si>
-    <t>https://octopart.com/dfe2hcah1r0mj0l-murata-100809337?r=sp</t>
-  </si>
-  <si>
-    <t>https://octopart.com/uclamp0501h.tct-semtech-587374?r=sp</t>
-  </si>
-  <si>
-    <t>https://octopart.com/ech8693r-tl-w-onsemi-30944216?r=sp</t>
-  </si>
-  <si>
     <t>https://octopart.com/max17330x22%2Bt-analog+devices-119633547?r=sp</t>
   </si>
   <si>
-    <t>https://octopart.com/tps631000drlr-texas+instruments-125396913?r=sp</t>
-  </si>
-  <si>
     <t>https://octopart.com/ld39200pu33r-stmicroelectronics-49646134?r=sp</t>
   </si>
   <si>
-    <t>R9, R15, R16, R17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tantalum Capacitors - Solid SMD 10V 22uF 3528 10% ESR=2.4ohms </t>
-  </si>
-  <si>
     <t>R2,R24</t>
   </si>
   <si>
@@ -574,24 +391,9 @@
     <t>https://octopart.com/vlmtg1300-gs08-vishay-21709202?r=sp</t>
   </si>
   <si>
-    <t>R5, R7, R8, R22</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C1, C2, C4, C6, C13</t>
-  </si>
-  <si>
     <t>CAP CER 0.1 UF 25V 10% X7R 0603</t>
   </si>
   <si>
-    <t>C0603C104Z3VACTU</t>
-  </si>
-  <si>
-    <t>https://octopart.com/c0603c104z3vactu-kemet-98662?r=sp</t>
-  </si>
-  <si>
     <t>5-146280-1</t>
   </si>
   <si>
@@ -604,9 +406,6 @@
     <t xml:space="preserve">1s Lipo charger w/ USB-C  (H05R0) </t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>2pin Terminal Block; Printed Circuit; 10 A; 160 V; 3.5 mm; 2; 3.5 mm; 1.2 mm; M2; PA</t>
   </si>
   <si>
@@ -629,13 +428,316 @@
   </si>
   <si>
     <t>D4</t>
+  </si>
+  <si>
+    <t>WFC12063L000FE66</t>
+  </si>
+  <si>
+    <t>RES 0.003 OHM 1.0 W 1% 1206 SMD</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>https://octopart.com/wfc12063l000fe66-vishay+dale-125245933?r=sp</t>
+  </si>
+  <si>
+    <t>R4, R6, R7, R10, R18</t>
+  </si>
+  <si>
+    <t>R22, R34</t>
+  </si>
+  <si>
+    <t>C9, C14</t>
+  </si>
+  <si>
+    <t>C1, C2, C4, C12, C13, C21, C22, C23, C24, C25, C26, C27, C31</t>
+  </si>
+  <si>
+    <t>C0805C475K4RACTU</t>
+  </si>
+  <si>
+    <t>KEMET [VA]</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c0805c475k4ractu-kemet-22859922?r=sp</t>
+  </si>
+  <si>
+    <t>CL10B104KA8NNNC</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cl10b104ka8nnnc-samsung-19831573?r=sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	C8, C32</t>
+  </si>
+  <si>
+    <t>C2012JB1V226M125AC</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c2012jb1v226m125ac-tdk-28168958?r=sp</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 22uF 35V JB 20% Pad SMD 0805 85C T/R</t>
+  </si>
+  <si>
+    <t>C10, C16</t>
+  </si>
+  <si>
+    <t>C0603C333K4RACTU</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c0603c333k4ractu-kemet-9143755?r=sp</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 0.033uF 16V X7R 10% SMD 1.6 x 0.8 mm 125 C Paper T/R</t>
+  </si>
+  <si>
+    <t>12401610E4#2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amphenol ICC </t>
+  </si>
+  <si>
+    <t>CONN RCP USB3.1 TYPEC 24P SMD RA</t>
+  </si>
+  <si>
+    <t>https://octopart.com/12401610e4%232a-amphenol+communications+solutions-126516878?r=sp</t>
+  </si>
+  <si>
+    <t>VBUS_OUT_J</t>
+  </si>
+  <si>
+    <t>B2P-VH-FB-B(LF)(SN)</t>
+  </si>
+  <si>
+    <t>https://octopart.com/b2p-vh-fb-b%28lf%29%28sn%29-jst-3990178?r=sp</t>
+  </si>
+  <si>
+    <t>VH Series 2 Position 3.96 mm Pitch Disconnectable Crimp Style Shrouded Header</t>
+  </si>
+  <si>
+    <t>BAT_J2</t>
+  </si>
+  <si>
+    <t>SISF06DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay </t>
+  </si>
+  <si>
+    <t>https://octopart.com/sisf06dn-t1-ge3-vishay-108916351?r=sp</t>
+  </si>
+  <si>
+    <t>Transistor MOSFET Array Dual N-CH 30V 28A 8-Pin PowerPAK 1212</t>
+  </si>
+  <si>
+    <t>TSV772IQ2T</t>
+  </si>
+  <si>
+    <t>https://octopart.com/tsv772iq2t-stmicroelectronics-123138659?r=sp</t>
+  </si>
+  <si>
+    <t>Op Amp Dual High Bandwidth Amplifier R-R I/O 5.5V 8-Pin DFN EP T/R</t>
+  </si>
+  <si>
+    <t>TS2431BILT</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ts2431bilt-stmicroelectronics-527041?r=sp</t>
+  </si>
+  <si>
+    <t>V-Ref Adjustable 2.5V to 24V 100mA 3-Pin SOT-23 T/R / IC VREF SHUNT ADJ SOT23-3</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>NCP45521IMNTWG-L</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ncp45521imntwg-l-onsemi-24638146?r=sp</t>
+  </si>
+  <si>
+    <t>0.5V~13.5V 12.8mΩ 10.5A DFN-8(2x2) Power Distribution Switches ROHS</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>LDK130C33R</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 300 mA 3.3 V Fixed Low Noise LDO Voltage Regulator - SOT-323-5</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ldk130c33r-stmicroelectronics-29288945?r=sp</t>
+  </si>
+  <si>
+    <t>D5, D6, D7</t>
+  </si>
+  <si>
+    <t>CUS10S30,H3F(T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toshiba </t>
+  </si>
+  <si>
+    <t>https://octopart.com/cus10s30%2Ch3f%28t-toshiba-98975237?r=sp</t>
+  </si>
+  <si>
+    <t>Schottky Diode, 30V, 1A, Sod-323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	R8, R20</t>
+  </si>
+  <si>
+    <t>RC0603FR-0749K9L</t>
+  </si>
+  <si>
+    <t>RES 49.9K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-0749k9l-yageo-1186134?r=sp</t>
+  </si>
+  <si>
+    <t>RC0603FR-0747KL</t>
+  </si>
+  <si>
+    <t>RES 47K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-0747kl-yageo-1369017?r=sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT_TH_J, PIO_J	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	R33</t>
+  </si>
+  <si>
+    <t>RC0603FR-072KL</t>
+  </si>
+  <si>
+    <t>RES THICK FILM 2K OHM 1/10W 1% 0603 SMD</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-072kl-yageo-39838380?r=sp</t>
+  </si>
+  <si>
+    <t>R35, R36</t>
+  </si>
+  <si>
+    <t>RMCF0603FG22K0</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rmcf0603fg22k0-stackpole+electronics-19773159?r=sp</t>
+  </si>
+  <si>
+    <t>0603 22K Ohm 1% 0.1W</t>
+  </si>
+  <si>
+    <t>R25, R28</t>
+  </si>
+  <si>
+    <t>RES SMD 220K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>0603WAJ0224T5E</t>
+  </si>
+  <si>
+    <t>ROYAL OHM</t>
+  </si>
+  <si>
+    <t>https://octopart.com/0603waj0224t5e-royal+ohm-127836159?r=sp</t>
+  </si>
+  <si>
+    <t>R27, R31</t>
+  </si>
+  <si>
+    <t>RC0603FR-0720KL</t>
+  </si>
+  <si>
+    <t>RES THICK FILM 20.0K OHM 1/10W 1% 0603 SMD</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-0720kl-yageo-1197359?r=sp</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>RC0603FR-071ML</t>
+  </si>
+  <si>
+    <t>RES 1M OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-071ml-yageo-1168402?r=sp</t>
+  </si>
+  <si>
+    <t>R3, R11, R21, R37, R39</t>
+  </si>
+  <si>
+    <t>08053D106KAT2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVX </t>
+  </si>
+  <si>
+    <t>https://octopart.com/08053d106kat2a-avx-71037153?r=sp</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 10uF 25V X5R 10% Pad SMD 0805</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>AC0603FR-0727KL</t>
+  </si>
+  <si>
+    <t>RES SMD 27K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ac0603fr-0727kl-yageo-28165829?r=sp</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R9, R15, R16, R17, R29</t>
+  </si>
+  <si>
+    <t>MCU 32-bit ARM Cortex M0+ RISC 512KB Flash 1.8V/2.5V/3.3V 48-Pin UFQFPN EP Tray</t>
+  </si>
+  <si>
+    <t>STM32G0B1CEU6</t>
+  </si>
+  <si>
+    <t>https://octopart.com/stm32g0b1ceu6-stmicroelectronics-116363364?r=sp</t>
+  </si>
+  <si>
+    <t>C19, C11, C15</t>
+  </si>
+  <si>
+    <t>C5, C6, C20, C28, C29, C30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -847,6 +949,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -1264,7 +1372,7 @@
     <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1335,6 +1443,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1752,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1800,7 +1911,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
@@ -1811,13 +1922,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="19">
-        <v>45213</v>
+        <v>45572</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="21"/>
@@ -1828,7 +1939,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>191</v>
+        <v>125</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1860,59 +1971,59 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>189</v>
+        <v>123</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>188</v>
+        <v>122</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="F9" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>115</v>
+        <v>196</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="F10" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>24</v>
       </c>
       <c r="F11" s="17">
         <v>1</v>
@@ -1920,99 +2031,99 @@
     </row>
     <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="F12" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="F13" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C14" s="15">
+      <c r="C14" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="15">
         <v>1984617</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="F14" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>58</v>
-      </c>
       <c r="D15" s="15" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="F15" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="F16" s="17">
         <v>1</v>
@@ -2020,379 +2131,379 @@
     </row>
     <row r="17" spans="1:6" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>100</v>
-      </c>
       <c r="C17" s="15" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="F17" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="F18" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>176</v>
+        <v>229</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="F19" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="F20" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F21" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>98</v>
+        <v>197</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F22" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>80</v>
-      </c>
       <c r="F23" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="F24" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>112</v>
+        <v>211</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>113</v>
+        <v>213</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>162</v>
+        <v>214</v>
       </c>
       <c r="F25" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>69</v>
+        <v>205</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>70</v>
+        <v>202</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>53</v>
+        <v>203</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>81</v>
+        <v>204</v>
       </c>
       <c r="F26" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>105</v>
+        <v>224</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>102</v>
+        <v>226</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>103</v>
+        <v>225</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>163</v>
+        <v>227</v>
       </c>
       <c r="F27" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>82</v>
+        <v>194</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>52</v>
+        <v>193</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>83</v>
+        <v>195</v>
       </c>
       <c r="F28" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F29" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>164</v>
+        <v>66</v>
       </c>
       <c r="F30" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>51</v>
+        <v>206</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>26</v>
+        <v>207</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>25</v>
+        <v>209</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>27</v>
+        <v>210</v>
       </c>
       <c r="F31" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>18</v>
+        <v>216</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>19</v>
+        <v>218</v>
       </c>
       <c r="F32" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B33" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>86</v>
-      </c>
       <c r="D33" s="15" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="F33" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>124</v>
+        <v>55</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>165</v>
+        <v>67</v>
       </c>
       <c r="F34" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="16" t="s">
         <v>111</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>166</v>
       </c>
       <c r="F35" s="17">
         <v>1</v>
@@ -2400,179 +2511,179 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F36" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="F37" s="17">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="F38" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>139</v>
+        <v>234</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="F39" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="F40" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>178</v>
+        <v>233</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>20</v>
+        <v>221</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>181</v>
+        <v>222</v>
       </c>
       <c r="F41" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>197</v>
+        <v>152</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>149</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>198</v>
+        <v>150</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>199</v>
+        <v>151</v>
       </c>
       <c r="F42" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>137</v>
+        <v>30</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>170</v>
+        <v>31</v>
       </c>
       <c r="F43" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="F44" s="17">
         <v>1</v>
@@ -2580,59 +2691,59 @@
     </row>
     <row r="45" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F45" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="F46" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="F47" s="17">
         <v>1</v>
@@ -2640,21 +2751,181 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>42</v>
+        <v>184</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="C48" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="F48" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="F49" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F50" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F48" s="17">
+      <c r="B51" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F52" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="F53" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F54" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="F55" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2665,23 +2936,39 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E23" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E26" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E28" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E31" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E33" r:id="rId11" display="https://octopart.com/grm21br61h106ke43k-murata-106705599?r=sp" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="E32" r:id="rId12" xr:uid="{CA2BC9B7-037F-4782-ACB8-2D8F29264691}"/>
-    <hyperlink ref="E39" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E38" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E21" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E30" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E34" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E44" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E43" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E17" r:id="rId10" xr:uid="{DD0ED2C5-E3EE-4C49-92C6-CED9241263EA}"/>
+    <hyperlink ref="E16" r:id="rId11" xr:uid="{7E429B88-FBBC-46BF-BA62-9500659DE8E5}"/>
+    <hyperlink ref="E39" r:id="rId12" xr:uid="{89A465E6-890C-483D-AF7F-2724481AADA7}"/>
+    <hyperlink ref="E37" r:id="rId13" xr:uid="{005DF22A-BCDD-4280-ABFA-613583E42166}"/>
+    <hyperlink ref="E42" r:id="rId14" xr:uid="{D51FF95F-FC5C-4E63-B570-AE86E94AA35F}"/>
+    <hyperlink ref="E36" r:id="rId15" xr:uid="{D7327B7B-E145-4FAB-8AD6-E71506C66BC9}"/>
+    <hyperlink ref="E14" r:id="rId16" xr:uid="{950DCE82-EF4F-4680-8608-03394FA2F301}"/>
+    <hyperlink ref="E13" r:id="rId17" xr:uid="{713826D7-23E7-47A1-AB22-C7082F38B03B}"/>
+    <hyperlink ref="E49" r:id="rId18" xr:uid="{EF8D19E3-A11A-45D2-90D3-E5A4997F450E}"/>
+    <hyperlink ref="E52" r:id="rId19" xr:uid="{820D286B-3E46-4ED1-9441-1D6956154609}"/>
+    <hyperlink ref="E45" r:id="rId20" xr:uid="{322A326E-EE9C-427D-A4F9-B305B217AE49}"/>
+    <hyperlink ref="E54" r:id="rId21" xr:uid="{B95262FF-2B2B-428E-A5BE-36D089F22DA3}"/>
+    <hyperlink ref="E55" r:id="rId22" xr:uid="{F9657CD2-697C-4E3C-8E2E-5B7B28AB704A}"/>
+    <hyperlink ref="E48" r:id="rId23" xr:uid="{290C7395-61B4-41E3-A917-974E387E3656}"/>
+    <hyperlink ref="E29" r:id="rId24" xr:uid="{FBCC4D9B-560E-47A5-BE32-2260A96B8C25}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{7B45AAC3-6E04-4EB5-BC94-C86AED9881D1}"/>
+    <hyperlink ref="E31" r:id="rId26" xr:uid="{5C3E4BAF-1579-463D-9C44-697E85034843}"/>
+    <hyperlink ref="E25" r:id="rId27" xr:uid="{F015B929-BC3E-444F-981F-C287AACE9D74}"/>
+    <hyperlink ref="E32" r:id="rId28" xr:uid="{119C8AD1-8BC7-4614-99C0-A76C7A2F7A27}"/>
+    <hyperlink ref="E41" r:id="rId29" xr:uid="{E2E21EC2-A7F8-4BEC-9250-7BEE71B657D3}"/>
+    <hyperlink ref="E50" r:id="rId30" xr:uid="{66D50468-75D1-4B70-81E6-4F1F3003E786}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>
-  <drawing r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId31"/>
+  <drawing r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>